<commit_message>
begin work on model
</commit_message>
<xml_diff>
--- a/Vent_Photon/datasheets/airflow model.xlsx
+++ b/Vent_Photon/datasheets/airflow model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="8328" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="8328" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Line Loss" sheetId="1" r:id="rId1"/>
@@ -257,7 +257,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -383,11 +382,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="489274184"/>
-        <c:axId val="489274576"/>
+        <c:axId val="495977136"/>
+        <c:axId val="495974000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="489274184"/>
+        <c:axId val="495977136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -444,12 +443,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="489274576"/>
+        <c:crossAx val="495974000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="489274576"/>
+        <c:axId val="495974000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -506,7 +505,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="489274184"/>
+        <c:crossAx val="495977136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -570,7 +569,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -658,7 +656,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -741,11 +738,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="489272616"/>
-        <c:axId val="489276928"/>
+        <c:axId val="495974784"/>
+        <c:axId val="495977528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="489272616"/>
+        <c:axId val="495974784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -802,12 +799,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="489276928"/>
+        <c:crossAx val="495977528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="489276928"/>
+        <c:axId val="495977528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -864,7 +861,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="489272616"/>
+        <c:crossAx val="495974784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1175,11 +1172,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="489276536"/>
-        <c:axId val="489277320"/>
+        <c:axId val="495975568"/>
+        <c:axId val="495980272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="489276536"/>
+        <c:axId val="495975568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1236,12 +1233,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="489277320"/>
+        <c:crossAx val="495980272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="489277320"/>
+        <c:axId val="495980272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1298,7 +1295,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="489276536"/>
+        <c:crossAx val="495975568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1362,6 +1359,86 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>ECMF-150</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> with 50' 6" Duct &amp; Filter</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1375,13 +1452,27 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1473,10 +1564,7 @@
                   <a:pPr>
                     <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
+                        <a:srgbClr val="0070C0"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -1642,8 +1730,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="489281240"/>
-        <c:axId val="489280064"/>
+        <c:axId val="495981056"/>
+        <c:axId val="495973608"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1686,6 +1774,54 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.7029746281714788E-3"/>
+                  <c:y val="0.36027777777777775"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.000E+00" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Model!$A$6:$A$26</c:f>
@@ -1840,11 +1976,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="489277712"/>
-        <c:axId val="489280848"/>
+        <c:axId val="496578520"/>
+        <c:axId val="418475008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="489281240"/>
+        <c:axId val="495981056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1901,12 +2037,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="489280064"/>
+        <c:crossAx val="495973608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="489280064"/>
+        <c:axId val="495973608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1963,12 +2099,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="489281240"/>
+        <c:crossAx val="495981056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="489280848"/>
+        <c:axId val="418475008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2011,12 +2147,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="489277712"/>
+        <c:crossAx val="496578520"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="489277712"/>
+        <c:axId val="496578520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2026,7 +2162,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="489280848"/>
+        <c:crossAx val="418475008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2122,6 +2258,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>ECMF-150 with 50' 6" Duct &amp; Filter</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2350,8 +2516,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="489282808"/>
-        <c:axId val="489279280"/>
+        <c:axId val="496582832"/>
+        <c:axId val="496585184"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2548,11 +2714,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="489279672"/>
-        <c:axId val="489283200"/>
+        <c:axId val="496588320"/>
+        <c:axId val="496587928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="489282808"/>
+        <c:axId val="496582832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2609,12 +2775,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="489279280"/>
+        <c:crossAx val="496585184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="489279280"/>
+        <c:axId val="496585184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2671,12 +2837,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="489282808"/>
+        <c:crossAx val="496582832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="489283200"/>
+        <c:axId val="496587928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2719,12 +2885,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="489279672"/>
+        <c:crossAx val="496588320"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="489279672"/>
+        <c:axId val="496588320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2734,7 +2900,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="489283200"/>
+        <c:crossAx val="496587928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2830,6 +2996,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Two Fans</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> in Series Same Duty Cycle</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -3110,8 +3306,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="492970008"/>
-        <c:axId val="492973928"/>
+        <c:axId val="496580088"/>
+        <c:axId val="496584008"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3308,11 +3504,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="492974712"/>
-        <c:axId val="492970792"/>
+        <c:axId val="496579304"/>
+        <c:axId val="496577736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="492970008"/>
+        <c:axId val="496580088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3369,12 +3565,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492973928"/>
+        <c:crossAx val="496584008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="492973928"/>
+        <c:axId val="496584008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3431,12 +3627,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492970008"/>
+        <c:crossAx val="496580088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="492970792"/>
+        <c:axId val="496577736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3479,12 +3675,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492974712"/>
+        <c:crossAx val="496579304"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="492974712"/>
+        <c:axId val="496579304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3494,7 +3690,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="492970792"/>
+        <c:crossAx val="496577736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3590,6 +3786,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Two Fans in Series Same Duty Cycle</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -3818,8 +4044,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="492975104"/>
-        <c:axId val="492976672"/>
+        <c:axId val="496588712"/>
+        <c:axId val="496585968"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -4016,11 +4242,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="492977064"/>
-        <c:axId val="492975888"/>
+        <c:axId val="496579696"/>
+        <c:axId val="496589104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="492975104"/>
+        <c:axId val="496588712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4077,12 +4303,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492976672"/>
+        <c:crossAx val="496585968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="492976672"/>
+        <c:axId val="496585968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4139,12 +4365,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492975104"/>
+        <c:crossAx val="496588712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="492975888"/>
+        <c:axId val="496589104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4187,12 +4413,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492977064"/>
+        <c:crossAx val="496579696"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="492977064"/>
+        <c:axId val="496579696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4202,7 +4428,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="492975888"/>
+        <c:crossAx val="496589104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8368,15 +8594,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
+      <xdr:colOff>251460</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8467,13 +8693,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>80010</xdr:rowOff>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>80010</xdr:rowOff>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9126,8 +9352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9843,8 +10069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>